<commit_message>
0530 crud ele proc
</commit_message>
<xml_diff>
--- a/중간발표/05.CRUD메트릭스.xlsx
+++ b/중간발표/05.CRUD메트릭스.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\데베설\git_corp\My-Cinema\중간발표\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF44C07-F6C2-4C1A-BAFF-36885BD75EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6225728-C1DC-4E87-B6E0-1C3655DA3FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{BF35880F-C2E3-41AF-9943-8008D55ED834}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="93">
   <si>
     <t>영화를 등록한다</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,10 +140,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>영화별 예매 방식으로 영화를 예매한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>영화를 영화이름으로 검색하여 조회한다(영화정보)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -228,10 +224,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>지역별 예매 방식으로 영화를 예매한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>회원의 시청 가능 여부를 확인한다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -393,6 +385,26 @@
   </si>
   <si>
     <t>U, C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원이 영화별 예매 방식으로 영화를 예매한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원이 지역별 예매 방식으로 영화를 예매한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비회원이 영화별 예매 방식으로 영화를 예매한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비회원이 지역별 예매 방식으로 영화를 예매한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>티켓을 조회한다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -400,7 +412,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,14 +430,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
@@ -433,17 +437,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -460,31 +459,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="나쁨" xfId="2" builtinId="27"/>
-    <cellStyle name="좋음" xfId="1" builtinId="26"/>
+  <cellStyles count="2">
+    <cellStyle name="나쁨" xfId="1" builtinId="27"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -797,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FCE492-328D-4B73-9660-E6C5C9C9FD95}">
-  <dimension ref="A1:AE47"/>
+  <dimension ref="A1:AE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -808,18 +800,22 @@
     <col min="1" max="1" width="7.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" customWidth="1"/>
+    <col min="5" max="6" width="7.125" customWidth="1"/>
+    <col min="7" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="5.25" customWidth="1"/>
+    <col min="10" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="11.75" customWidth="1"/>
+    <col min="13" max="13" width="7.125" customWidth="1"/>
+    <col min="14" max="14" width="5.25" customWidth="1"/>
+    <col min="15" max="15" width="7.125" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="15.125" customWidth="1"/>
+    <col min="19" max="23" width="9" customWidth="1"/>
+    <col min="24" max="24" width="13" customWidth="1"/>
+    <col min="25" max="25" width="5.875" customWidth="1"/>
+    <col min="26" max="27" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
@@ -845,19 +841,19 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="M1" t="s">
         <v>15</v>
       </c>
       <c r="N1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P1" t="s">
         <v>16</v>
@@ -866,62 +862,62 @@
         <v>17</v>
       </c>
       <c r="R1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" t="s">
         <v>52</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>53</v>
       </c>
-      <c r="V1" t="s">
-        <v>54</v>
-      </c>
-      <c r="W1" t="s">
-        <v>55</v>
-      </c>
       <c r="X1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Y1" t="s">
         <v>18</v>
       </c>
       <c r="Z1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AA1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AB1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AC1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>66</v>
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
-        <v>67</v>
+      <c r="C3" t="s">
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -929,10 +925,10 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -942,8 +938,8 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
-        <v>69</v>
+      <c r="C5" t="s">
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -951,10 +947,10 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -967,8 +963,8 @@
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C7" s="1" t="s">
-        <v>71</v>
+      <c r="C7" t="s">
+        <v>69</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
@@ -976,26 +972,26 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
         <v>72</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C10" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="G10" t="s">
         <v>22</v>
@@ -1003,26 +999,26 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
         <v>75</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C12" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C13" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="Z13" t="s">
         <v>22</v>
@@ -1030,9 +1026,9 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
         <v>0</v>
       </c>
       <c r="I14" t="s">
@@ -1049,7 +1045,7 @@
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="F15" t="s">
@@ -1070,10 +1066,10 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
         <v>45</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
@@ -1083,8 +1079,8 @@
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C17" s="1" t="s">
-        <v>47</v>
+      <c r="C17" t="s">
+        <v>46</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
@@ -1092,9 +1088,9 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="F18" t="s">
@@ -1105,7 +1101,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>3</v>
       </c>
       <c r="H19" t="s">
@@ -1114,40 +1110,40 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="N20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="S21" t="s">
+        <v>20</v>
+      </c>
+      <c r="X21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>20</v>
+      </c>
+      <c r="R22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
         <v>86</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="N20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S21" t="s">
-        <v>20</v>
-      </c>
-      <c r="X21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>20</v>
-      </c>
-      <c r="R22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C23" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="M23" t="s">
         <v>21</v>
@@ -1158,12 +1154,12 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="M25" t="s">
@@ -1177,7 +1173,7 @@
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="N26" t="s">
@@ -1185,7 +1181,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="M27" t="s">
@@ -1199,7 +1195,7 @@
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>24</v>
       </c>
       <c r="N28" t="s">
@@ -1210,7 +1206,7 @@
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>25</v>
       </c>
       <c r="Q29" t="s">
@@ -1222,64 +1218,64 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" t="s">
+        <v>20</v>
+      </c>
+      <c r="L30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="I30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" t="s">
-        <v>20</v>
-      </c>
-      <c r="K30" t="s">
-        <v>20</v>
-      </c>
-      <c r="L30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C31" s="1" t="s">
+      <c r="I31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" t="s">
+        <v>20</v>
+      </c>
+      <c r="P31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
         <v>28</v>
-      </c>
-      <c r="I31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J31" t="s">
-        <v>20</v>
-      </c>
-      <c r="K31" t="s">
-        <v>20</v>
-      </c>
-      <c r="L31" t="s">
-        <v>20</v>
-      </c>
-      <c r="P31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I32" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" t="s">
-        <v>20</v>
-      </c>
-      <c r="K32" t="s">
-        <v>20</v>
-      </c>
-      <c r="L32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C33" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="I33" t="s">
         <v>20</v>
@@ -1296,224 +1292,248 @@
     </row>
     <row r="34" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" t="s">
+        <v>20</v>
+      </c>
+      <c r="N34" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" t="s">
+        <v>20</v>
+      </c>
+      <c r="O35" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" t="s">
+        <v>20</v>
+      </c>
+      <c r="M38" t="s">
+        <v>19</v>
+      </c>
+      <c r="O38" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" t="s">
+        <v>20</v>
+      </c>
+      <c r="I39" t="s">
+        <v>20</v>
+      </c>
+      <c r="K39" t="s">
+        <v>20</v>
+      </c>
+      <c r="M39" t="s">
+        <v>19</v>
+      </c>
+      <c r="O39" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="M40" t="s">
+        <v>21</v>
+      </c>
+      <c r="O40" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" t="s">
-        <v>20</v>
-      </c>
-      <c r="K34" t="s">
-        <v>20</v>
-      </c>
-      <c r="M34" t="s">
-        <v>19</v>
-      </c>
-      <c r="O34" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C35" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35" t="s">
-        <v>20</v>
-      </c>
-      <c r="K35" t="s">
-        <v>20</v>
-      </c>
-      <c r="M35" t="s">
-        <v>19</v>
-      </c>
-      <c r="O35" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z35" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I36" t="s">
-        <v>20</v>
-      </c>
-      <c r="N36" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" t="s">
-        <v>20</v>
-      </c>
-      <c r="O37" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C38" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M38" t="s">
-        <v>21</v>
-      </c>
-      <c r="O38" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB38" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="C41" t="s">
+        <v>54</v>
+      </c>
+      <c r="S41" t="s">
+        <v>19</v>
+      </c>
+      <c r="T41" t="s">
+        <v>20</v>
+      </c>
+      <c r="U41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>55</v>
+      </c>
+      <c r="S42" t="s">
+        <v>19</v>
+      </c>
+      <c r="T42" t="s">
+        <v>20</v>
+      </c>
+      <c r="V42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
         <v>56</v>
       </c>
-      <c r="S39" t="s">
-        <v>19</v>
-      </c>
-      <c r="T39" t="s">
-        <v>20</v>
-      </c>
-      <c r="U39" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C40" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="S40" t="s">
-        <v>19</v>
-      </c>
-      <c r="T40" t="s">
-        <v>20</v>
-      </c>
-      <c r="V40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C41" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="S41" t="s">
-        <v>19</v>
-      </c>
-      <c r="T41" t="s">
-        <v>20</v>
-      </c>
-      <c r="W41" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N42" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>19</v>
-      </c>
-      <c r="R42" t="s">
-        <v>19</v>
-      </c>
-      <c r="S42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L43" t="s">
-        <v>22</v>
-      </c>
       <c r="S43" t="s">
-        <v>20</v>
-      </c>
-      <c r="X43" t="s">
+        <v>19</v>
+      </c>
+      <c r="T43" t="s">
+        <v>20</v>
+      </c>
+      <c r="W43" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="44" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>40</v>
       </c>
       <c r="N44" t="s">
@@ -1525,58 +1545,92 @@
       <c r="R44" t="s">
         <v>19</v>
       </c>
-      <c r="X44" t="s">
-        <v>20</v>
+      <c r="S44" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C45" s="1" t="s">
-        <v>43</v>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="L45" t="s">
+        <v>22</v>
       </c>
       <c r="S45" t="s">
         <v>20</v>
       </c>
       <c r="X45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
+        <v>39</v>
+      </c>
+      <c r="N46" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>19</v>
+      </c>
+      <c r="R46" t="s">
+        <v>19</v>
+      </c>
+      <c r="X46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" t="s">
         <v>42</v>
       </c>
-      <c r="L46" t="s">
+      <c r="S47" t="s">
+        <v>20</v>
+      </c>
+      <c r="X47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>41</v>
+      </c>
+      <c r="L48" t="s">
         <v>22</v>
       </c>
-      <c r="Q46" t="s">
-        <v>19</v>
-      </c>
-      <c r="R46" t="s">
-        <v>19</v>
-      </c>
-      <c r="S46" t="s">
-        <v>20</v>
-      </c>
-      <c r="X46" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C47" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>20</v>
-      </c>
-      <c r="R47" t="s">
-        <v>20</v>
-      </c>
-      <c r="S47" t="s">
-        <v>20</v>
-      </c>
-      <c r="X47" t="s">
+      <c r="Q48" t="s">
+        <v>19</v>
+      </c>
+      <c r="R48" t="s">
+        <v>87</v>
+      </c>
+      <c r="S48" t="s">
+        <v>20</v>
+      </c>
+      <c r="X48" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>20</v>
+      </c>
+      <c r="R49" t="s">
+        <v>20</v>
+      </c>
+      <c r="S49" t="s">
+        <v>20</v>
+      </c>
+      <c r="X49" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>